<commit_message>
Balance now shows on Profile page. From and To usernames now included in Transaction record.
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -101,7 +101,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -166,9 +166,9 @@
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -631,7 +631,7 @@
         <v>-91.5</v>
       </c>
       <c r="K5" s="1" t="str">
-        <f t="shared" ref="K5:M5" si="0">IF(J5&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="K5" si="0">IF(J5&gt;=0, "CR", "DB")</f>
         <v>DB</v>
       </c>
       <c r="L5" s="1">
@@ -686,7 +686,7 @@
         <v>-66.5</v>
       </c>
       <c r="K6" s="1" t="str">
-        <f t="shared" ref="K6:M8" si="3">IF(J6&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="K6:K8" si="3">IF(J6&gt;=0, "CR", "DB")</f>
         <v>DB</v>
       </c>
       <c r="L6" s="1">
@@ -828,7 +828,7 @@
         <v>-41.5</v>
       </c>
       <c r="K9" s="1" t="str">
-        <f t="shared" ref="K9:M9" si="9">IF(J9&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="K9" si="9">IF(J9&gt;=0, "CR", "DB")</f>
         <v>DB</v>
       </c>
       <c r="L9" s="1">
@@ -836,7 +836,7 @@
         <v>66.5</v>
       </c>
       <c r="M9" s="1" t="str">
-        <f t="shared" ref="M9:O9" si="11">IF(L9&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="M9" si="11">IF(L9&gt;=0, "CR", "DB")</f>
         <v>CR</v>
       </c>
       <c r="N9" s="1">
@@ -844,7 +844,7 @@
         <v>-25</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" ref="O9:P9" si="13">IF(N9&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="O9" si="13">IF(N9&gt;=0, "CR", "DB")</f>
         <v>DB</v>
       </c>
       <c r="P9" s="4">
@@ -871,7 +871,7 @@
         <v>-41.5</v>
       </c>
       <c r="K10" s="1" t="str">
-        <f t="shared" ref="K10:M10" si="15">IF(J10&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="K10" si="15">IF(J10&gt;=0, "CR", "DB")</f>
         <v>DB</v>
       </c>
       <c r="L10" s="1">
@@ -879,7 +879,7 @@
         <v>66.5</v>
       </c>
       <c r="M10" s="1" t="str">
-        <f t="shared" ref="M10:O10" si="16">IF(L10&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="M10" si="16">IF(L10&gt;=0, "CR", "DB")</f>
         <v>CR</v>
       </c>
       <c r="N10" s="1">
@@ -887,7 +887,7 @@
         <v>-25</v>
       </c>
       <c r="O10" s="1" t="str">
-        <f t="shared" ref="O10:P10" si="17">IF(N10&gt;=0, "CR", "DB")</f>
+        <f t="shared" ref="O10" si="17">IF(N10&gt;=0, "CR", "DB")</f>
         <v>DB</v>
       </c>
       <c r="P10" s="4">

</xml_diff>

<commit_message>
Transactions now have title and names included in record. Title shown on transaction list. Add payment FAB added onto profile page.
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,22 +547,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>5.5</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
         <f>IF(C4=$F$3, B4, IF(D4=$F$3, (B4*-1), 0))</f>
-        <v>5.5</v>
+        <v>-97</v>
       </c>
       <c r="G4" s="1">
         <f>IF(C4=$G$3, B4, IF(D4=$G$3, (B4*-1), 0))</f>
-        <v>-5.5</v>
+        <v>97</v>
       </c>
       <c r="H4" s="1">
         <f>IF(C4=$H$3, B4, IF(D4=$H$3, (B4*-1), 0))</f>
@@ -570,19 +570,19 @@
       </c>
       <c r="J4" s="1">
         <f>F4</f>
-        <v>5.5</v>
+        <v>-97</v>
       </c>
       <c r="K4" s="1" t="str">
         <f>IF(J4&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="L4" s="1">
         <f>G4</f>
-        <v>-5.5</v>
+        <v>97</v>
       </c>
       <c r="M4" s="1" t="str">
         <f>IF(L4&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="N4" s="1">
         <f>H4</f>
@@ -604,23 +604,21 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
-        <v>97</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
         <f>IF(C5=$F$3, B5, IF(D5=$F$3, (B5*-1), 0))</f>
-        <v>-97</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <f>IF(C5=$G$3, B5, IF(D5=$G$3, (B5*-1), 0))</f>
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1">
         <f>IF(C5=$H$3, B5, IF(D5=$H$3, (B5*-1), 0))</f>
@@ -628,7 +626,7 @@
       </c>
       <c r="J5" s="1">
         <f>J4+F5</f>
-        <v>-91.5</v>
+        <v>-97</v>
       </c>
       <c r="K5" s="1" t="str">
         <f t="shared" ref="K5" si="0">IF(J5&gt;=0, "CR", "DB")</f>
@@ -636,7 +634,7 @@
       </c>
       <c r="L5" s="1">
         <f>L4+G5</f>
-        <v>91.5</v>
+        <v>97</v>
       </c>
       <c r="M5" s="1" t="str">
         <f t="shared" ref="M5:O5" si="1">IF(L5&gt;=0, "CR", "DB")</f>
@@ -659,9 +657,7 @@
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
-        <v>25</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
@@ -671,11 +667,11 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <f>IF(C6=$F$3, B6, IF(D6=$F$3, (B6*-1), 0))</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <f>IF(C6=$G$3, B6, IF(D6=$G$3, (B6*-1), 0))</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <f>IF(C6=$H$3, B6, IF(D6=$H$3, (B6*-1), 0))</f>
@@ -683,7 +679,7 @@
       </c>
       <c r="J6" s="1">
         <f>J5+F6</f>
-        <v>-66.5</v>
+        <v>-97</v>
       </c>
       <c r="K6" s="1" t="str">
         <f t="shared" ref="K6:K8" si="3">IF(J6&gt;=0, "CR", "DB")</f>
@@ -691,7 +687,7 @@
       </c>
       <c r="L6" s="1">
         <f>L5+G6</f>
-        <v>66.5</v>
+        <v>97</v>
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" ref="M6:O8" si="4">IF(L6&gt;=0, "CR", "DB")</f>
@@ -715,9 +711,7 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>25</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
@@ -726,7 +720,7 @@
       </c>
       <c r="F7" s="1">
         <f>IF(C7=$F$3, B7, IF(D7=$F$3, (B7*-1), 0))</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
         <f>IF(C7=$G$3, B7, IF(D7=$G$3, (B7*-1), 0))</f>
@@ -734,11 +728,11 @@
       </c>
       <c r="H7" s="1">
         <f>IF(C7=$H$3, B7, IF(D7=$H$3, (B7*-1), 0))</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1">
         <f>J6+F7</f>
-        <v>-41.5</v>
+        <v>-97</v>
       </c>
       <c r="K7" s="1" t="str">
         <f t="shared" si="3"/>
@@ -746,7 +740,7 @@
       </c>
       <c r="L7" s="1">
         <f>L6+G7</f>
-        <v>66.5</v>
+        <v>97</v>
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="4"/>
@@ -754,11 +748,11 @@
       </c>
       <c r="N7" s="1">
         <f>N6+H7</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="2"/>
@@ -781,7 +775,7 @@
       </c>
       <c r="J8" s="1">
         <f>J7+F8</f>
-        <v>-41.5</v>
+        <v>-97</v>
       </c>
       <c r="K8" s="1" t="str">
         <f t="shared" si="3"/>
@@ -789,7 +783,7 @@
       </c>
       <c r="L8" s="1">
         <f>L7+G8</f>
-        <v>66.5</v>
+        <v>97</v>
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="4"/>
@@ -797,11 +791,11 @@
       </c>
       <c r="N8" s="1">
         <f>N7+H8</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="2"/>
@@ -825,7 +819,7 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ref="J9:J10" si="8">J8+F9</f>
-        <v>-41.5</v>
+        <v>-97</v>
       </c>
       <c r="K9" s="1" t="str">
         <f t="shared" ref="K9" si="9">IF(J9&gt;=0, "CR", "DB")</f>
@@ -833,7 +827,7 @@
       </c>
       <c r="L9" s="1">
         <f t="shared" ref="L9:L10" si="10">L8+G9</f>
-        <v>66.5</v>
+        <v>97</v>
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" ref="M9" si="11">IF(L9&gt;=0, "CR", "DB")</f>
@@ -841,11 +835,11 @@
       </c>
       <c r="N9" s="1">
         <f t="shared" ref="N9:N10" si="12">N8+H9</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" ref="O9" si="13">IF(N9&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" ref="P9:P10" si="14">SUM(N9+L9+J9)</f>
@@ -868,7 +862,7 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" si="8"/>
-        <v>-41.5</v>
+        <v>-97</v>
       </c>
       <c r="K10" s="1" t="str">
         <f t="shared" ref="K10" si="15">IF(J10&gt;=0, "CR", "DB")</f>
@@ -876,7 +870,7 @@
       </c>
       <c r="L10" s="1">
         <f t="shared" si="10"/>
-        <v>66.5</v>
+        <v>97</v>
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" ref="M10" si="16">IF(L10&gt;=0, "CR", "DB")</f>
@@ -884,11 +878,11 @@
       </c>
       <c r="N10" s="1">
         <f t="shared" si="12"/>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="O10" s="1" t="str">
         <f t="shared" ref="O10" si="17">IF(N10&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="P10" s="4">
         <f t="shared" si="14"/>
@@ -932,7 +926,7 @@
     <row r="16" spans="1:17">
       <c r="B16" s="6">
         <f>IF(AND(C4="Alan", D4="Neady"), B4, IF(AND(C4="Neady", D4="Alan"), B4*-1,0))</f>
-        <v>5.5</v>
+        <v>-97</v>
       </c>
       <c r="C16" s="6">
         <f>IF(AND(C4="Alan", D4="Nick"), B4, IF(AND(C4="Nick", D4="Alan"), B4*-1,0))</f>
@@ -946,10 +940,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="B17" s="6">
         <f>IF(AND(C5="Alan", D5="Neady"), B5, IF(AND(C5="Neady", D5="Alan"), B5*-1,0))</f>
-        <v>-97</v>
+        <v>0</v>
       </c>
       <c r="C17" s="6">
         <f>IF(AND(C5="Alan", D5="Nick"), B5, IF(AND(C5="Nick", D5="Alan"), B5*-1,0))</f>
@@ -963,10 +957,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="B18" s="6">
         <f>IF(AND(C6="Alan", D6="Neady"), B6, IF(AND(C6="Neady", D6="Alan"), B6*-1,0))</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C18" s="6">
         <f>IF(AND(C6="Alan", D6="Nick"), B6, IF(AND(C6="Nick", D6="Alan"), B6*-1,0))</f>
@@ -980,18 +974,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="B19" s="6">
         <f>IF(AND(C7="Alan", D7="Neady"), B7, IF(AND(C7="Neady", D7="Alan"), B7*-1,0))</f>
         <v>0</v>
       </c>
       <c r="C19" s="6">
         <f>IF(AND(C7="Alan", D7="Nick"), B7, IF(AND(C7="Nick", D7="Alan"), B7*-1,0))</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="B20" s="6">
         <f>IF(AND(C8="Alan", D8="Neady"), B8, IF(AND(C8="Neady", D8="Alan"), B8*-1,0))</f>
         <v>0</v>
@@ -1001,8 +995,11 @@
         <v>0</v>
       </c>
       <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="B21" s="6">
         <f t="shared" ref="B21:B22" si="18">IF(AND(C9="Alan", D9="Neady"), B9, IF(AND(C9="Neady", D9="Alan"), B9*-1,0))</f>
         <v>0</v>
@@ -1012,8 +1009,11 @@
         <v>0</v>
       </c>
       <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="B22" s="6">
         <f t="shared" si="18"/>
         <v>0</v>
@@ -1023,36 +1023,39 @@
         <v>0</v>
       </c>
       <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="B24" s="8">
         <f>SUM(B16:B22)</f>
-        <v>-66.5</v>
+        <v>-97</v>
       </c>
       <c r="C24" s="8">
         <f>SUM(C16:C22)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D24" s="8">
         <f>SUM(B24:C24)</f>
-        <v>-41.5</v>
+        <v>-97</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>IF(D24&gt;=0, "CR", "DB")</f>
         <v>DB</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -1060,7 +1063,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
         <v>19</v>
@@ -1070,10 +1073,10 @@
       </c>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="B28" s="6">
         <f>IF(AND(C4="Neady", D4="Alan"), B4, IF(AND(C4="Alan", D4="Neady"), B4*-1,0))</f>
-        <v>-5.5</v>
+        <v>97</v>
       </c>
       <c r="C28" s="6">
         <f>IF(AND(C4="Neady", D4="Nick"), B4, IF(AND(C4="Nick", D4="Neady"), B4*-1,0))</f>
@@ -1081,10 +1084,10 @@
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="B29" s="6">
         <f>IF(AND(C5="Neady", D5="Alan"), B5, IF(AND(C5="Alan", D5="Neady"), B5*-1,0))</f>
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="C29" s="6">
         <f>IF(AND(C5="Neady", D5="Nick"), B5, IF(AND(C5="Nick", D5="Neady"), B5*-1,0))</f>
@@ -1092,10 +1095,10 @@
       </c>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="B30" s="6">
         <f>IF(AND(C6="Neady", D6="Alan"), B6, IF(AND(C6="Alan", D6="Neady"), B6*-1,0))</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="C30" s="6">
         <f>IF(AND(C6="Neady", D6="Nick"), B6, IF(AND(C6="Nick", D6="Neady"), B6*-1,0))</f>
@@ -1103,7 +1106,7 @@
       </c>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="B31" s="6">
         <f>IF(AND(C7="Neady", D7="Alan"), B7, IF(AND(C7="Alan", D7="Neady"), B7*-1,0))</f>
         <v>0</v>
@@ -1114,7 +1117,7 @@
       </c>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:10">
       <c r="B32" s="6">
         <f>IF(AND(C8="Neady", D8="Alan"), B8, IF(AND(C8="Alan", D8="Neady"), B8*-1,0))</f>
         <v>0</v>
@@ -1155,7 +1158,7 @@
     <row r="36" spans="1:5">
       <c r="B36" s="8">
         <f>SUM(B28:B34)</f>
-        <v>66.5</v>
+        <v>97</v>
       </c>
       <c r="C36" s="8">
         <f>SUM(C28:C34)</f>
@@ -1163,7 +1166,7 @@
       </c>
       <c r="D36" s="8">
         <f>SUM(B36:C36)</f>
-        <v>66.5</v>
+        <v>97</v>
       </c>
       <c r="E36" s="1" t="str">
         <f>IF(D36&gt;=0, "CR", "DB")</f>
@@ -1229,7 +1232,7 @@
     <row r="43" spans="1:5">
       <c r="B43" s="6">
         <f>IF(AND(C7="Nick", D7="Alan"), B7, IF(AND(C7="Alan", D7="Nick"), B7*-1,0))</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="C43" s="6">
         <f>IF(AND(C7="Nick", D7="Neady"), B7, IF(AND(C7="Neady", D7="Nick"), B7*-1,0))</f>
@@ -1278,7 +1281,7 @@
     <row r="48" spans="1:5">
       <c r="B48" s="8">
         <f>SUM(B40:B46)</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="C48" s="8">
         <f>SUM(C40:C46)</f>
@@ -1286,11 +1289,11 @@
       </c>
       <c r="D48" s="8">
         <f>SUM(B48:C48)</f>
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="E48" s="1" t="str">
         <f>IF(D48&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balances moved from balances node into each users node. Balance field added to signupUser in auth-data.ts. New balances fields now updated in updateFirebaseAfterTicketsBought() in EventData. Balance in profile now getting value from correct place in Firebase.
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,22 +547,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>97</v>
+        <v>5.5</v>
       </c>
       <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
         <f>IF(C4=$F$3, B4, IF(D4=$F$3, (B4*-1), 0))</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="G4" s="1">
         <f>IF(C4=$G$3, B4, IF(D4=$G$3, (B4*-1), 0))</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="H4" s="1">
         <f>IF(C4=$H$3, B4, IF(D4=$H$3, (B4*-1), 0))</f>
@@ -570,19 +570,19 @@
       </c>
       <c r="J4" s="1">
         <f>F4</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="K4" s="1" t="str">
         <f>IF(J4&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="L4" s="1">
         <f>G4</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="M4" s="1" t="str">
         <f>IF(L4&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="N4" s="1">
         <f>H4</f>
@@ -606,10 +606,10 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
@@ -626,19 +626,19 @@
       </c>
       <c r="J5" s="1">
         <f>J4+F5</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="K5" s="1" t="str">
         <f t="shared" ref="K5" si="0">IF(J5&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="L5" s="1">
         <f>L4+G5</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="M5" s="1" t="str">
         <f t="shared" ref="M5:O5" si="1">IF(L5&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="N5" s="1">
         <f>N4+H5</f>
@@ -679,19 +679,19 @@
       </c>
       <c r="J6" s="1">
         <f>J5+F6</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="K6" s="1" t="str">
         <f t="shared" ref="K6:K8" si="3">IF(J6&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="L6" s="1">
         <f>L5+G6</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" ref="M6:O8" si="4">IF(L6&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="N6" s="1">
         <f>N5+H6</f>
@@ -732,19 +732,19 @@
       </c>
       <c r="J7" s="1">
         <f>J6+F7</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="K7" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="L7" s="1">
         <f>L6+G7</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="N7" s="1">
         <f>N6+H7</f>
@@ -775,19 +775,19 @@
       </c>
       <c r="J8" s="1">
         <f>J7+F8</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="K8" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="L8" s="1">
         <f>L7+G8</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="N8" s="1">
         <f>N7+H8</f>
@@ -819,19 +819,19 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ref="J9:J10" si="8">J8+F9</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="K9" s="1" t="str">
         <f t="shared" ref="K9" si="9">IF(J9&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" ref="L9:L10" si="10">L8+G9</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" ref="M9" si="11">IF(L9&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" ref="N9:N10" si="12">N8+H9</f>
@@ -862,19 +862,19 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" si="8"/>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="K10" s="1" t="str">
         <f t="shared" ref="K10" si="15">IF(J10&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="10"/>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" ref="M10" si="16">IF(L10&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="12"/>
@@ -926,7 +926,7 @@
     <row r="16" spans="1:17">
       <c r="B16" s="6">
         <f>IF(AND(C4="Alan", D4="Neady"), B4, IF(AND(C4="Neady", D4="Alan"), B4*-1,0))</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="C16" s="6">
         <f>IF(AND(C4="Alan", D4="Nick"), B4, IF(AND(C4="Nick", D4="Alan"), B4*-1,0))</f>
@@ -1035,7 +1035,7 @@
     <row r="24" spans="1:10">
       <c r="B24" s="8">
         <f>SUM(B16:B22)</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="C24" s="8">
         <f>SUM(C16:C22)</f>
@@ -1043,11 +1043,11 @@
       </c>
       <c r="D24" s="8">
         <f>SUM(B24:C24)</f>
-        <v>-97</v>
+        <v>5.5</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>IF(D24&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1076,7 +1076,7 @@
     <row r="28" spans="1:10">
       <c r="B28" s="6">
         <f>IF(AND(C4="Neady", D4="Alan"), B4, IF(AND(C4="Alan", D4="Neady"), B4*-1,0))</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="C28" s="6">
         <f>IF(AND(C4="Neady", D4="Nick"), B4, IF(AND(C4="Nick", D4="Neady"), B4*-1,0))</f>
@@ -1158,7 +1158,7 @@
     <row r="36" spans="1:5">
       <c r="B36" s="8">
         <f>SUM(B28:B34)</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="C36" s="8">
         <f>SUM(C28:C34)</f>
@@ -1166,11 +1166,11 @@
       </c>
       <c r="D36" s="8">
         <f>SUM(B36:C36)</f>
-        <v>97</v>
+        <v>-5.5</v>
       </c>
       <c r="E36" s="1" t="str">
         <f>IF(D36&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
     </row>
     <row r="37" spans="1:5">

</xml_diff>

<commit_message>
Transaction datetime now the same for all transactions for one event.
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -604,7 +604,9 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>97</v>
+      </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -614,11 +616,11 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1">
         <f>IF(C5=$F$3, B5, IF(D5=$F$3, (B5*-1), 0))</f>
-        <v>0</v>
+        <v>-97</v>
       </c>
       <c r="G5" s="1">
         <f>IF(C5=$G$3, B5, IF(D5=$G$3, (B5*-1), 0))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1">
         <f>IF(C5=$H$3, B5, IF(D5=$H$3, (B5*-1), 0))</f>
@@ -626,19 +628,19 @@
       </c>
       <c r="J5" s="1">
         <f>J4+F5</f>
-        <v>5.5</v>
+        <v>-91.5</v>
       </c>
       <c r="K5" s="1" t="str">
         <f t="shared" ref="K5" si="0">IF(J5&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="L5" s="1">
         <f>L4+G5</f>
-        <v>-5.5</v>
+        <v>91.5</v>
       </c>
       <c r="M5" s="1" t="str">
         <f t="shared" ref="M5:O5" si="1">IF(L5&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="N5" s="1">
         <f>N4+H5</f>
@@ -657,7 +659,9 @@
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>25</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
@@ -667,11 +671,11 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <f>IF(C6=$F$3, B6, IF(D6=$F$3, (B6*-1), 0))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1">
         <f>IF(C6=$G$3, B6, IF(D6=$G$3, (B6*-1), 0))</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="H6" s="1">
         <f>IF(C6=$H$3, B6, IF(D6=$H$3, (B6*-1), 0))</f>
@@ -679,19 +683,19 @@
       </c>
       <c r="J6" s="1">
         <f>J5+F6</f>
-        <v>5.5</v>
+        <v>-66.5</v>
       </c>
       <c r="K6" s="1" t="str">
         <f t="shared" ref="K6:K8" si="3">IF(J6&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="L6" s="1">
         <f>L5+G6</f>
-        <v>-5.5</v>
+        <v>66.5</v>
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" ref="M6:O8" si="4">IF(L6&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="N6" s="1">
         <f>N5+H6</f>
@@ -711,7 +715,9 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
@@ -720,7 +726,7 @@
       </c>
       <c r="F7" s="1">
         <f>IF(C7=$F$3, B7, IF(D7=$F$3, (B7*-1), 0))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1">
         <f>IF(C7=$G$3, B7, IF(D7=$G$3, (B7*-1), 0))</f>
@@ -728,31 +734,31 @@
       </c>
       <c r="H7" s="1">
         <f>IF(C7=$H$3, B7, IF(D7=$H$3, (B7*-1), 0))</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="J7" s="1">
         <f>J6+F7</f>
-        <v>5.5</v>
+        <v>-41.5</v>
       </c>
       <c r="K7" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="L7" s="1">
         <f>L6+G7</f>
-        <v>-5.5</v>
+        <v>66.5</v>
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="N7" s="1">
         <f>N6+H7</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="2"/>
@@ -775,27 +781,27 @@
       </c>
       <c r="J8" s="1">
         <f>J7+F8</f>
-        <v>5.5</v>
+        <v>-41.5</v>
       </c>
       <c r="K8" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="L8" s="1">
         <f>L7+G8</f>
-        <v>-5.5</v>
+        <v>66.5</v>
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="N8" s="1">
         <f>N7+H8</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="2"/>
@@ -819,27 +825,27 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ref="J9:J10" si="8">J8+F9</f>
-        <v>5.5</v>
+        <v>-41.5</v>
       </c>
       <c r="K9" s="1" t="str">
         <f t="shared" ref="K9" si="9">IF(J9&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" ref="L9:L10" si="10">L8+G9</f>
-        <v>-5.5</v>
+        <v>66.5</v>
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" ref="M9" si="11">IF(L9&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" ref="N9:N10" si="12">N8+H9</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" ref="O9" si="13">IF(N9&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" ref="P9:P10" si="14">SUM(N9+L9+J9)</f>
@@ -862,27 +868,27 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" si="8"/>
-        <v>5.5</v>
+        <v>-41.5</v>
       </c>
       <c r="K10" s="1" t="str">
         <f t="shared" ref="K10" si="15">IF(J10&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="10"/>
-        <v>-5.5</v>
+        <v>66.5</v>
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" ref="M10" si="16">IF(L10&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="O10" s="1" t="str">
         <f t="shared" ref="O10" si="17">IF(N10&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
       <c r="P10" s="4">
         <f t="shared" si="14"/>
@@ -943,7 +949,7 @@
     <row r="17" spans="1:10">
       <c r="B17" s="6">
         <f>IF(AND(C5="Alan", D5="Neady"), B5, IF(AND(C5="Neady", D5="Alan"), B5*-1,0))</f>
-        <v>0</v>
+        <v>-97</v>
       </c>
       <c r="C17" s="6">
         <f>IF(AND(C5="Alan", D5="Nick"), B5, IF(AND(C5="Nick", D5="Alan"), B5*-1,0))</f>
@@ -960,7 +966,7 @@
     <row r="18" spans="1:10">
       <c r="B18" s="6">
         <f>IF(AND(C6="Alan", D6="Neady"), B6, IF(AND(C6="Neady", D6="Alan"), B6*-1,0))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C18" s="6">
         <f>IF(AND(C6="Alan", D6="Nick"), B6, IF(AND(C6="Nick", D6="Alan"), B6*-1,0))</f>
@@ -981,7 +987,7 @@
       </c>
       <c r="C19" s="6">
         <f>IF(AND(C7="Alan", D7="Nick"), B7, IF(AND(C7="Nick", D7="Alan"), B7*-1,0))</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D19" s="7"/>
     </row>
@@ -1035,19 +1041,19 @@
     <row r="24" spans="1:10">
       <c r="B24" s="8">
         <f>SUM(B16:B22)</f>
-        <v>5.5</v>
+        <v>-66.5</v>
       </c>
       <c r="C24" s="8">
         <f>SUM(C16:C22)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D24" s="8">
         <f>SUM(B24:C24)</f>
-        <v>5.5</v>
+        <v>-41.5</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>IF(D24&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1087,7 +1093,7 @@
     <row r="29" spans="1:10">
       <c r="B29" s="6">
         <f>IF(AND(C5="Neady", D5="Alan"), B5, IF(AND(C5="Alan", D5="Neady"), B5*-1,0))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="C29" s="6">
         <f>IF(AND(C5="Neady", D5="Nick"), B5, IF(AND(C5="Nick", D5="Neady"), B5*-1,0))</f>
@@ -1098,7 +1104,7 @@
     <row r="30" spans="1:10">
       <c r="B30" s="6">
         <f>IF(AND(C6="Neady", D6="Alan"), B6, IF(AND(C6="Alan", D6="Neady"), B6*-1,0))</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="C30" s="6">
         <f>IF(AND(C6="Neady", D6="Nick"), B6, IF(AND(C6="Nick", D6="Neady"), B6*-1,0))</f>
@@ -1158,7 +1164,7 @@
     <row r="36" spans="1:5">
       <c r="B36" s="8">
         <f>SUM(B28:B34)</f>
-        <v>-5.5</v>
+        <v>66.5</v>
       </c>
       <c r="C36" s="8">
         <f>SUM(C28:C34)</f>
@@ -1166,11 +1172,11 @@
       </c>
       <c r="D36" s="8">
         <f>SUM(B36:C36)</f>
-        <v>-5.5</v>
+        <v>66.5</v>
       </c>
       <c r="E36" s="1" t="str">
         <f>IF(D36&gt;=0, "CR", "DB")</f>
-        <v>DB</v>
+        <v>CR</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1232,7 +1238,7 @@
     <row r="43" spans="1:5">
       <c r="B43" s="6">
         <f>IF(AND(C7="Nick", D7="Alan"), B7, IF(AND(C7="Alan", D7="Nick"), B7*-1,0))</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="C43" s="6">
         <f>IF(AND(C7="Nick", D7="Neady"), B7, IF(AND(C7="Neady", D7="Nick"), B7*-1,0))</f>
@@ -1281,7 +1287,7 @@
     <row r="48" spans="1:5">
       <c r="B48" s="8">
         <f>SUM(B40:B46)</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="C48" s="8">
         <f>SUM(C40:C46)</f>
@@ -1289,11 +1295,11 @@
       </c>
       <c r="D48" s="8">
         <f>SUM(B48:C48)</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="E48" s="1" t="str">
         <f>IF(D48&gt;=0, "CR", "DB")</f>
-        <v>CR</v>
+        <v>DB</v>
       </c>
     </row>
   </sheetData>

</xml_diff>